<commit_message>
Trying some plots and correlations
</commit_message>
<xml_diff>
--- a/report/HCI/Self Assessment Form - HCI.xlsx
+++ b/report/HCI/Self Assessment Form - HCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\HCI-TWEB_2025-26\report\HCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1633871C-0E12-453D-86A8-0378E3BBEB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54D1AC5-674F-4B03-A12F-D54A7EFA84E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>please do not modify the form; do not introduce new columns; do not introduce new rows; we will process the form automatically!!</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Huge datasets could be a challenge in terms of cleaning (e.g. Dropping duplicates in different buckets, needed not to saturate RAM, is not possible)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>https://gitlab2.educ.di.unito.it/st182487/HCI-TWEB_2025-26</t>
+  </si>
+  <si>
+    <t>NaN values are skipped automatically from Pandas so we don't need to throw specific exceptions</t>
   </si>
 </sst>
 </file>
@@ -675,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -811,11 +820,15 @@
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
@@ -885,7 +898,7 @@
       <c r="Y13" s="22"/>
       <c r="Z13" s="22"/>
     </row>
-    <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="96" x14ac:dyDescent="0.4">
       <c r="A14" s="23"/>
       <c r="B14" s="4" t="s">
         <v>14</v>
@@ -900,7 +913,10 @@
         <v>15</v>
       </c>
       <c r="D15" s="14">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -936,7 +952,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -945,7 +961,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -977,7 +993,7 @@
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -987,7 +1003,7 @@
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -997,7 +1013,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1007,7 +1023,7 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1287,7 +1303,7 @@
         <v>46</v>
       </c>
       <c r="D62" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1296,7 +1312,7 @@
         <v>47</v>
       </c>
       <c r="D63" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -5096,6 +5112,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some tweaks and more plots+story
</commit_message>
<xml_diff>
--- a/report/HCI/Self Assessment Form - HCI.xlsx
+++ b/report/HCI/Self Assessment Form - HCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\HCI-TWEB_2025-26\report\HCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54D1AC5-674F-4B03-A12F-D54A7EFA84E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24718F7E-15B8-4F55-9E57-68C007FD34BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>please do not modify the form; do not introduce new columns; do not introduce new rows; we will process the form automatically!!</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>NaN values are skipped automatically from Pandas so we don't need to throw specific exceptions</t>
+  </si>
+  <si>
+    <t>Could have used more python classes and modules to make the code reusable and modular</t>
+  </si>
+  <si>
+    <t>Some results may be incorrect due to the lack of values and/or not so reliable ones</t>
+  </si>
+  <si>
+    <t>It already handles millions of records, though for very large dataset a more powerful machine may be needed</t>
   </si>
 </sst>
 </file>
@@ -684,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -904,7 +913,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -925,7 +934,10 @@
         <v>16</v>
       </c>
       <c r="D16" s="14">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1150,7 +1162,10 @@
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="14">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1170,7 +1185,10 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="14">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Adding new plots and adjusting some of the already written cells
</commit_message>
<xml_diff>
--- a/report/HCI/Self Assessment Form - HCI.xlsx
+++ b/report/HCI/Self Assessment Form - HCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\HCI-TWEB_2025-26\report\HCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24718F7E-15B8-4F55-9E57-68C007FD34BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF27B6-2A88-4071-BB7D-E23AB60A5F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -323,6 +323,14 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -390,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -476,9 +484,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1142,7 +1151,7 @@
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1152,7 +1161,7 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1175,7 +1184,7 @@
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1235,7 +1244,7 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1296,6 +1305,7 @@
       <c r="C57" s="10" t="s">
         <v>44</v>
       </c>
+      <c r="D57" s="39"/>
     </row>
     <row r="58" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="23"/>
@@ -1397,8 +1407,12 @@
       <c r="A72" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
+      <c r="B72" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C72" s="25">
+        <v>0.5</v>
+      </c>
       <c r="D72" s="25"/>
     </row>
     <row r="73" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Final tweaks one my side
</commit_message>
<xml_diff>
--- a/report/HCI/Self Assessment Form - HCI.xlsx
+++ b/report/HCI/Self Assessment Form - HCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\HCI-TWEB_2025-26\report\HCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF27B6-2A88-4071-BB7D-E23AB60A5F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E879F-EA53-495B-B5E4-D1E9684EC9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>please do not modify the form; do not introduce new columns; do not introduce new rows; we will process the form automatically!!</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>It already handles millions of records, though for very large dataset a more powerful machine may be needed</t>
+  </si>
+  <si>
+    <t>Cleaned roughly half the .csv files containing data, analyzed and created plots and insights regarding the datasets</t>
+  </si>
+  <si>
+    <t>Every difficult-to-understand line of code is well commented. Though, there's room for improvement. The report is described to understand the main steps done during the assignment</t>
   </si>
 </sst>
 </file>
@@ -475,6 +481,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -484,7 +491,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -702,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -717,12 +723,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -747,12 +753,12 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1254,7 +1260,7 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1264,7 +1270,7 @@
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1274,7 +1280,7 @@
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1284,7 +1290,7 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1294,7 +1300,7 @@
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1305,7 +1311,7 @@
       <c r="C57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D57" s="39"/>
+      <c r="D57" s="34"/>
     </row>
     <row r="58" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="23"/>
@@ -1350,6 +1356,9 @@
       </c>
       <c r="C64" s="10" t="s">
         <v>48</v>
+      </c>
+      <c r="D64" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1399,8 +1408,12 @@
       <c r="A71" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
+      <c r="B71" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="D71" s="25"/>
     </row>
     <row r="72" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Refactored the HCI part and finished with the report
</commit_message>
<xml_diff>
--- a/report/HCI/Self Assessment Form - HCI.xlsx
+++ b/report/HCI/Self Assessment Form - HCI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\HCI-TWEB_2025-26\report\HCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E879F-EA53-495B-B5E4-D1E9684EC9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E748C570-5B1B-45AA-AC6A-AC74E9E08F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>please do not modify the form; do not introduce new columns; do not introduce new rows; we will process the form automatically!!</t>
   </si>
@@ -232,6 +232,36 @@
   </si>
   <si>
     <t>Every difficult-to-understand line of code is well commented. Though, there's room for improvement. The report is described to understand the main steps done during the assignment</t>
+  </si>
+  <si>
+    <t>The code was organized in a modular way inside the Jupyter notebook by clearly separating different phases of the work.
+Data loading, data cleaning, feature creation, and analysis were kept in separate sections and cells, following a logical pipeline.
+Even though all the code is contained in the notebook, each step performs a specific task and does not mix preprocessing with analysis or visualization.
+This makes the notebook easy to read, debug, and modify, and allows focusing on one operation at a time.
+Pandas was used extensively to perform efficient data analysis through vectorized operations.
+Functions such as groupby, value_counts, merge, and datetime handling allowed us to process large datasets and extract trends in a concise and readable way without using explicit loops.</t>
+  </si>
+  <si>
+    <t>The original datasets contain missing values, inconsistent formats, and some ambiguous entries, so specific cleaning rules were needed to make the data usable.
+Because the datasets are very large, memory usage was an important concern, and some operations (such as dropping duplicates across chunks) were not feasible without risking RAM saturation.
+We decided to rely on standard Pandas functions for simplicity and reliability, while optimizing the data loading process.
+This included converting columns to more memory-efficient types (for example, using category instead of strings) and selecting only the necessary columns with the usecols parameter.
+A specific issue involved a user with a null username in both the profiles and ratings datasets.
+Replacing this value would have broken the link between the datasets, so the row was dropped to avoid ambiguity.</t>
+  </si>
+  <si>
+    <t>The data analytics strategy was based on asking clear questions and exploring the data step by step.
+Each analysis focused on a specific aspect of the dataset, such as time trends, user behavior, or relationships between variables.
+We paid attention to data quality, filtering out outliers and poorly represented cases to avoid misleading results.
+When needed, data was grouped or aggregated to highlight meaningful patterns instead of random noise.
+This approach is effective because it combines numerical analysis with critical reasoning, not just data processing.</t>
+  </si>
+  <si>
+    <t>The visualization strategy follows the principles taught in the module, focusing on clarity, readability, and purpose.
+Each chart was chosen based on the type of data and the question being answered, trying to avoid unnecessary complexity (even though sometimes we didn't manage to).
+When visualizations became too dense, we simplified them by aggregating data or splitting the analysis into multiple plots.
+Interactivity was used when useful to help compare many categories without overwhelming the viewer.
+Overall, the visualizations are effective because they support the analysis and help communicate insights clearly to non-technical users.</t>
   </si>
 </sst>
 </file>
@@ -404,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -481,7 +511,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -491,6 +520,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -708,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="77" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -723,12 +758,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -753,12 +788,12 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -999,7 +1034,9 @@
       <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="25"/>
+      <c r="D23" s="25" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="23"/>
@@ -1137,6 +1174,9 @@
       <c r="C39" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="D39" s="39" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="23"/>
@@ -1213,7 +1253,7 @@
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1223,7 +1263,7 @@
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1234,6 +1274,9 @@
       <c r="C49" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="D49" s="39" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="23" t="s">
@@ -1311,7 +1354,9 @@
       <c r="C57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D57" s="34"/>
+      <c r="D57" s="40" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="23"/>

</xml_diff>